<commit_message>
An excel file with graphs and statistics on sorting has been completed. And fixed the design of the laboratory in accordance with google c++ style
</commit_message>
<xml_diff>
--- a/statistics/data.xlsx
+++ b/statistics/data.xlsx
@@ -73,15 +73,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,12 +101,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -9982,16 +10012,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>165735</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>603885</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>165735</xdr:rowOff>
+      <xdr:colOff>299085</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10279,7 +10309,7 @@
   <dimension ref="A1:C152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M152" sqref="M152"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10290,1368 +10320,1368 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>1000</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>251647</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>501317</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2000</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1004916</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>2005864</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3000</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2258393</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>4510828</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4000</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4014394</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>8020839</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5000</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>6278355</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>12546772</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6000</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>9055026</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>18098123</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7000</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>12302880</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>24591842</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8000</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>16116926</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>32217944</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9000</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>20350381</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>40682865</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10000</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>25181847</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>50343807</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>25000</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>156986620</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>313923504</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>50000</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>628139906</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>1256180325</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>1000</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>11672</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>15835</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>2000</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>28797</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>42662</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>3000</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>51171</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>79488</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>4000</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>78140</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>125478</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>5000</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>110324</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>182661</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>6000</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>147574</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>248941</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>7000</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>188791</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>323887</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>8000</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>236992</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>412862</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>9000</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>288584</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>506974</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>10000</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>345436</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>612651</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>25000</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>1801337</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>3405606</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>50000</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>6709271</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>13021407</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>1000</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>8703</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>19952</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>2000</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>19404</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>43904</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>3000</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>30904</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>69808</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>4000</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>42801</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>95808</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>5000</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>55185</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>123616</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>6000</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>67792</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>151616</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>7000</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>80621</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>179616</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>8000</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>93572</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>207616</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>9000</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>106893</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>237232</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>10000</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>120349</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>267232</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>25000</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>333777</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>734464</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>50000</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>717421</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="2">
         <v>1568928</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>1000</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="2">
         <f>A51-1</f>
         <v>999</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>2000</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="2">
         <f t="shared" ref="B52:B63" si="0">A52-1</f>
         <v>1999</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>3000</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="2">
         <f t="shared" si="0"/>
         <v>2999</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>4000</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="2">
         <f t="shared" si="0"/>
         <v>3999</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>5000</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="2">
         <f t="shared" si="0"/>
         <v>4999</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>6000</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="2">
         <f t="shared" si="0"/>
         <v>5999</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>7000</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="2">
         <f t="shared" si="0"/>
         <v>6999</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>8000</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="2">
         <f t="shared" si="0"/>
         <v>7999</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>9000</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="2">
         <f t="shared" si="0"/>
         <v>8999</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>10000</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="2">
         <f t="shared" si="0"/>
         <v>9999</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>25000</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="2">
         <f t="shared" si="0"/>
         <v>24999</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="2">
         <v>50000</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="2">
         <f t="shared" si="0"/>
         <v>49999</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="2">
         <v>100000</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="2">
         <f t="shared" si="0"/>
         <v>99999</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67">
+      <c r="A67" s="2">
         <v>1000</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="2">
         <v>499500</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="2">
         <v>999000</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68">
+      <c r="A68" s="2">
         <v>2000</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="2">
         <v>1999000</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="2">
         <v>3998000</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69">
+      <c r="A69" s="2">
         <v>3000</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="2">
         <v>4498500</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="2">
         <v>8997000</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70">
+      <c r="A70" s="2">
         <v>4000</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="2">
         <v>7998000</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="2">
         <v>15996000</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71">
+      <c r="A71" s="2">
         <v>5000</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="2">
         <v>12497500</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="2">
         <v>24995000</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72">
+      <c r="A72" s="2">
         <v>6000</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="2">
         <v>17997000</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="2">
         <v>35994000</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73">
+      <c r="A73" s="2">
         <v>7000</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="2">
         <v>24496500</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="2">
         <v>48993000</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74">
+      <c r="A74" s="2">
         <v>8000</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="2">
         <v>31996000</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="2">
         <v>63992000</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75">
+      <c r="A75" s="2">
         <v>9000</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="2">
         <v>40495500</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="2">
         <v>80991000</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76">
+      <c r="A76" s="2">
         <v>10000</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="2">
         <v>49995000</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="2">
         <v>99990000</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77">
+      <c r="A77" s="2">
         <v>25000</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="2">
         <v>312487500</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="2">
         <v>624975000</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78">
+      <c r="A78" s="2">
         <v>50000</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="2">
         <v>1249975000</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="2">
         <v>2499950000</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79">
+      <c r="A79" s="2">
         <v>100000</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="2">
         <v>4999950000</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="2">
         <v>9999900000</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="A86" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="A87" s="2">
         <v>1000</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="2">
         <v>499500</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="2">
         <v>1000998</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="A88" s="2">
         <v>2000</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="2">
         <v>1999000</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="2">
         <v>4001998</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="A89" s="2">
         <v>3000</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="2">
         <v>4498500</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="2">
         <v>9002998</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="A90" s="2">
         <v>4000</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="2">
         <v>7998000</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="2">
         <v>16003998</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="A91" s="2">
         <v>5000</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="2">
         <v>12497500</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="2">
         <v>25004998</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="A92" s="2">
         <v>6000</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="2">
         <v>17997000</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="2">
         <v>36005998</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93">
+      <c r="A93" s="2">
         <v>7000</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="2">
         <v>24496500</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="2">
         <v>49006998</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="A94" s="2">
         <v>8000</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="2">
         <v>31996000</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="2">
         <v>64007998</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="A95" s="2">
         <v>9000</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="2">
         <v>40495500</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="2">
         <v>81008998</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96">
+      <c r="A96" s="2">
         <v>10000</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="2">
         <v>49995000</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="2">
         <v>99990000</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="A97" s="2">
         <v>25000</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="2">
         <v>312487500</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="2">
         <v>624975000</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="A98" s="2">
         <v>50000</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="2">
         <v>1249975000</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="2">
         <v>2499950000</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="A99" s="2">
         <v>100000</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="2">
         <v>4999950000</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="2">
         <v>9999900000</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="A104" s="2">
         <v>1000</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="2">
         <v>499500</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="2">
         <v>500998</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105">
+      <c r="A105" s="2">
         <v>2000</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="2">
         <v>1999000</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="2">
         <v>2001998</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106">
+      <c r="A106" s="2">
         <v>3000</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="2">
         <v>4498500</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="2">
         <v>4502998</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107">
+      <c r="A107" s="2">
         <v>4000</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="2">
         <v>7998000</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="2">
         <v>12504998</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108">
+      <c r="A108" s="2">
         <v>5000</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="2">
         <v>12497500</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="2">
         <v>12504998</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109">
+      <c r="A109" s="2">
         <v>6000</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="2">
         <v>17997000</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="2">
         <v>18005998</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110">
+      <c r="A110" s="2">
         <v>7000</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="2">
         <v>24496500</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="2">
         <v>24506998</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111">
+      <c r="A111" s="2">
         <v>8000</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="2">
         <v>31996000</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="2">
         <v>32007998</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112">
+      <c r="A112" s="2">
         <v>9000</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="2">
         <v>40495500</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="2">
         <v>40508998</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113">
+      <c r="A113" s="2">
         <v>10000</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="2">
         <v>49995000</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="2">
         <v>99990000</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114">
+      <c r="A114" s="2">
         <v>25000</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="2">
         <v>312487500</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="2">
         <v>624975000</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115">
+      <c r="A115" s="2">
         <v>50000</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="2">
         <v>1249975000</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="2">
         <v>2499950000</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116">
+      <c r="A116" s="2">
         <v>100000</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="2">
         <v>4999950000</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="2">
         <v>9999900000</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121">
+      <c r="A121" s="2">
         <v>1000</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="2">
         <v>5044</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="2">
         <v>19952</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122">
+      <c r="A122" s="2">
         <v>2000</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="2">
         <v>11088</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="2">
         <v>43904</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123">
+      <c r="A123" s="2">
         <v>3000</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="2">
         <v>18076</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="2">
         <v>69808</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124">
+      <c r="A124" s="2">
         <v>4000</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="2">
         <v>24176</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="2">
         <v>95808</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125">
+      <c r="A125" s="2">
         <v>5000</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="2">
         <v>32004</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="2">
         <v>123616</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126">
+      <c r="A126" s="2">
         <v>6000</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="2">
         <v>39152</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="2">
         <v>151616</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127">
+      <c r="A127" s="2">
         <v>7000</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="2">
         <v>46180</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="2">
         <v>179616</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128">
+      <c r="A128" s="2">
         <v>8000</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="2">
         <v>52352</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="2">
         <v>207616</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129">
+      <c r="A129" s="2">
         <v>9000</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="2">
         <v>60796</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="2">
         <v>237232</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130">
+      <c r="A130" s="2">
         <v>10000</v>
       </c>
-      <c r="B130">
+      <c r="B130" s="2">
         <v>69008</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="2">
         <v>267232</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131">
+      <c r="A131" s="2">
         <v>25000</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="2">
         <v>188476</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="2">
         <v>734464</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132">
+      <c r="A132" s="2">
         <v>50000</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="2">
         <v>401952</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="2">
         <v>1568928</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133">
+      <c r="A133" s="2">
         <v>100000</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="2">
         <v>853904</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="2">
         <v>3337856</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+      <c r="A139" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140">
+      <c r="A140" s="2">
         <v>1000</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="2">
         <v>4932</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="2">
         <v>19952</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141">
+      <c r="A141" s="2">
         <v>2000</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="2">
         <v>10864</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="2">
         <v>43904</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142">
+      <c r="A142" s="2">
         <v>3000</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="2">
         <v>16828</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="2">
         <v>69808</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143">
+      <c r="A143" s="2">
         <v>4000</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="2">
         <v>23728</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="2">
         <v>95808</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144">
+      <c r="A144" s="2">
         <v>5000</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="2">
         <v>29804</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="2">
         <v>123616</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145">
+      <c r="A145" s="2">
         <v>6000</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="2">
         <v>36656</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="2">
         <v>151616</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146">
+      <c r="A146" s="2">
         <v>7000</v>
       </c>
-      <c r="B146">
+      <c r="B146" s="2">
         <v>43628</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="2">
         <v>179616</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147">
+      <c r="A147" s="2">
         <v>8000</v>
       </c>
-      <c r="B147">
+      <c r="B147" s="2">
         <v>51456</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="2">
         <v>207616</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148">
+      <c r="A148" s="2">
         <v>9000</v>
       </c>
-      <c r="B148">
+      <c r="B148" s="2">
         <v>57820</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="2">
         <v>237232</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149">
+      <c r="A149" s="2">
         <v>10000</v>
       </c>
-      <c r="B149">
+      <c r="B149" s="2">
         <v>64608</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="2">
         <v>267232</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150">
+      <c r="A150" s="2">
         <v>25000</v>
       </c>
-      <c r="B150">
+      <c r="B150" s="2">
         <v>178756</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="2">
         <v>734464</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151">
+      <c r="A151" s="2">
         <v>50000</v>
       </c>
-      <c r="B151">
+      <c r="B151" s="2">
         <v>382512</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="2">
         <v>1568928</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152">
+      <c r="A152" s="2">
         <v>100000</v>
       </c>
-      <c r="B152">
+      <c r="B152" s="2">
         <v>815024</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="2">
         <v>3337856</v>
       </c>
     </row>

</xml_diff>